<commit_message>
Updated Headers, created CSV for easy import
</commit_message>
<xml_diff>
--- a/Datasets/Freddie_Mac_15_Year_30_Year_Interest_Rate.xlsx
+++ b/Datasets/Freddie_Mac_15_Year_30_Year_Interest_Rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea8e7c1a7f050da2/Documents/GitHub/project-one/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{D95284D4-A948-4786-B017-71330B9B4B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7AFA550-A3E6-427C-ADD5-4AD5EB271979}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{D95284D4-A948-4786-B017-71330B9B4B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{031B17F6-26BF-45E4-8213-026DCF29682B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{92484BE9-355B-44B8-975A-569F6C3BC6FB}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>15_Year_Annual_Average_Rate</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>https://www.freddiemac.com/pmms/pmms30</t>
+  </si>
+  <si>
+    <t>Observation_Date</t>
   </si>
 </sst>
 </file>
@@ -75,6 +75,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -433,9 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B8F73-83BD-43B1-91B7-2896497E6D4F}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -828,25 +827,25 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="25.5">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:6" ht="25.5">
       <c r="A2" s="2">
         <v>40544</v>
       </c>
@@ -863,7 +862,7 @@
         <v>0.7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5">
@@ -883,7 +882,7 @@
         <v>0.7</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5">
@@ -903,7 +902,7 @@
         <v>0.7</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25.5">
@@ -923,7 +922,7 @@
         <v>0.6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5">
@@ -943,7 +942,7 @@
         <v>0.6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5">
@@ -963,7 +962,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5">
@@ -983,7 +982,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5">
@@ -1003,7 +1002,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="25.5">
@@ -1023,7 +1022,7 @@
         <v>0.52916666666666667</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.5">
@@ -1043,7 +1042,7 @@
         <v>0.73499999999999988</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="25.5">
@@ -1063,7 +1062,7 @@
         <v>0.69166666666666676</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>